<commit_message>
modified:   "Result/2022\353\205\2043\354\233\224 \354\266\225\354\242\205\353\263\204 \353\217\204\353\247\244(\355\217\211\352\267\240\352\260\200\352\262\251).xlsx"
</commit_message>
<xml_diff>
--- a/Result/2022년3월 축종별 도매(평균가격).xlsx
+++ b/Result/2022년3월 축종별 도매(평균가격).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyf13\Desktop\test\Price prediction\Result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyf13\Desktop\test\Price-prediction\Result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8445DC1E-2E6E-4916-A511-E26E8E64C7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318230B4-215A-4E98-934B-EDD3ADB4D6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3936" yWindow="252" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>일자</t>
   </si>
@@ -35,18 +35,41 @@
   <si>
     <t>지육가격(한우)(원/kg)</t>
   </si>
+  <si>
+    <t>2023년 3월 도매(평균가격) 예측 결과</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="휴먼명조"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="휴먼명조"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -57,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -65,22 +88,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -363,372 +413,383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:E34"/>
+  <dimension ref="C2:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
+    <row r="2" spans="3:5" ht="18">
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="3:5" ht="35">
+      <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C4" s="4">
+    <row r="4" spans="3:5" ht="18">
+      <c r="C4" s="7">
         <v>44986</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="8">
         <v>17992.828028075899</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="8">
         <v>4669.0427107056603</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" s="4">
+    <row r="5" spans="3:5" ht="18">
+      <c r="C5" s="7">
         <v>44987</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="8">
         <v>18079.333660423799</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="8">
         <v>4809.1710639255098</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="4">
+    <row r="6" spans="3:5" ht="18">
+      <c r="C6" s="7">
         <v>44988</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="8">
         <v>18124.739055121001</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="8">
         <v>4771.5214377744696</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="4">
+    <row r="7" spans="3:5" ht="18">
+      <c r="C7" s="7">
         <v>44989</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="8">
         <v>17905.362986422198</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="8">
         <v>4663.6505436007101</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="4">
+    <row r="8" spans="3:5" ht="18">
+      <c r="C8" s="7">
         <v>44990</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="8">
         <v>18487.828787837399</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="8">
         <v>4531.3838473532296</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="4">
+    <row r="9" spans="3:5" ht="18">
+      <c r="C9" s="7">
         <v>44991</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="8">
         <v>19182.096406844601</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="8">
         <v>4516.0584877300198</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="4">
+    <row r="10" spans="3:5" ht="18">
+      <c r="C10" s="7">
         <v>44992</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="8">
         <v>15417.495550403901</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="8">
         <v>4399.8349530503401</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="4">
+    <row r="11" spans="3:5" ht="18">
+      <c r="C11" s="7">
         <v>44993</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="8">
         <v>18614.343629440202</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="8">
         <v>4398.0417574081002</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="4">
+    <row r="12" spans="3:5" ht="18">
+      <c r="C12" s="7">
         <v>44994</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="8">
         <v>19171.971766877901</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="8">
         <v>4474.0067937705999</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="4">
+    <row r="13" spans="3:5" ht="18">
+      <c r="C13" s="7">
         <v>44995</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="8">
         <v>19176.0340479101</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="8">
         <v>4542.35301551258</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C14" s="4">
+    <row r="14" spans="3:5" ht="18">
+      <c r="C14" s="7">
         <v>44996</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="8">
         <v>20031.996745470198</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="8">
         <v>4571.1883832498397</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C15" s="4">
+    <row r="15" spans="3:5" ht="18">
+      <c r="C15" s="7">
         <v>44997</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="8">
         <v>19564.6701325309</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="8">
         <v>4693.8965790109196</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C16" s="4">
+    <row r="16" spans="3:5" ht="18">
+      <c r="C16" s="7">
         <v>44998</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="8">
         <v>19025.632774269499</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="8">
         <v>4727.5957088142004</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="4">
+    <row r="17" spans="3:5" ht="18">
+      <c r="C17" s="7">
         <v>44999</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="8">
         <v>15860.773153628201</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="8">
         <v>4703.9525699388496</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="4">
+    <row r="18" spans="3:5" ht="18">
+      <c r="C18" s="7">
         <v>45000</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="8">
         <v>19744.8478658321</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="8">
         <v>4749.3447660105203</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="4">
+    <row r="19" spans="3:5" ht="18">
+      <c r="C19" s="7">
         <v>45001</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="8">
         <v>19933.932737559498</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="8">
         <v>4562.7812821862299</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="4">
+    <row r="20" spans="3:5" ht="18">
+      <c r="C20" s="7">
         <v>45002</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="8">
         <v>19529.618401047999</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="8">
         <v>4654.8317671065097</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="4">
+    <row r="21" spans="3:5" ht="18">
+      <c r="C21" s="7">
         <v>45003</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="8">
         <v>19198.775354619698</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="8">
         <v>4689.4870338066303</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C22" s="4">
+    <row r="22" spans="3:5" ht="18">
+      <c r="C22" s="7">
         <v>45004</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="8">
         <v>19248.539883550999</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="8">
         <v>4883.2126947768102</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C23" s="4">
+    <row r="23" spans="3:5" ht="18">
+      <c r="C23" s="7">
         <v>45005</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="8">
         <v>14129.169077157099</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="8">
         <v>4815.51148553449</v>
       </c>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C24" s="4">
+    <row r="24" spans="3:5" ht="18">
+      <c r="C24" s="7">
         <v>45006</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="8">
         <v>19740.569630292899</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="8">
         <v>4778.8359524499801</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C25" s="4">
+    <row r="25" spans="3:5" ht="18">
+      <c r="C25" s="7">
         <v>45007</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="8">
         <v>19617.720151230202</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="8">
         <v>4993.6281552356704</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C26" s="4">
+    <row r="26" spans="3:5" ht="18">
+      <c r="C26" s="7">
         <v>45008</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="8">
         <v>17678.408225046402</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="8">
         <v>5021.4048773532804</v>
       </c>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C27" s="4">
+    <row r="27" spans="3:5" ht="18">
+      <c r="C27" s="7">
         <v>45009</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="8">
         <v>20761.931921818799</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="8">
         <v>5144.1130731143503</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C28" s="4">
+    <row r="28" spans="3:5" ht="18">
+      <c r="C28" s="7">
         <v>45010</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="8">
         <v>21229.653663964302</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="8">
         <v>5177.8122029176402</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C29" s="4">
+    <row r="29" spans="3:5" ht="18">
+      <c r="C29" s="7">
         <v>45011</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="8">
         <v>21169.8034361225</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="8">
         <v>5154.1690640422903</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C30" s="4">
+    <row r="30" spans="3:5" ht="18">
+      <c r="C30" s="7">
         <v>45012</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="8">
         <v>20973.886772441601</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="8">
         <v>5199.5612601139601</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C31" s="4">
+    <row r="31" spans="3:5" ht="18">
+      <c r="C31" s="7">
         <v>45013</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="8">
         <v>16437.6149996364</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="8">
         <v>5012.9977762896697</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C32" s="4">
+    <row r="32" spans="3:5" ht="18">
+      <c r="C32" s="7">
         <v>45014</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="8">
         <v>20365.517989062198</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="8">
         <v>5105.0482612099404</v>
       </c>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C33" s="4">
+    <row r="33" spans="3:5" ht="18">
+      <c r="C33" s="7">
         <v>45015</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="8">
         <v>20216.3792571583</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="8">
         <v>5139.7035279100701</v>
       </c>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C34" s="4">
+    <row r="34" spans="3:5" ht="18">
+      <c r="C34" s="7">
         <v>45016</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="8">
         <v>18383.0504876263</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="8">
         <v>5333.42918888025</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>